<commit_message>
Updated info on hall sheet
</commit_message>
<xml_diff>
--- a/Barker College/IP Register Barker.xlsx
+++ b/Barker College/IP Register Barker.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\code\Barker College\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\Precision-Code\Barker College\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="721" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="721"/>
   </bookViews>
   <sheets>
     <sheet name="PROJECT CENTRE" sheetId="16" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="178">
   <si>
     <t>Device</t>
   </si>
@@ -554,6 +554,15 @@
   </si>
   <si>
     <t>Programmer patch port - F</t>
+  </si>
+  <si>
+    <t>Barker Guest Wifi - can see AV VLAN</t>
+  </si>
+  <si>
+    <t>pi@barker</t>
+  </si>
+  <si>
+    <t>Added Wifi Details in the hall sheet</t>
   </si>
 </sst>
 </file>
@@ -911,7 +920,7 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -1122,41 +1131,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1210,7 +1222,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 2"/>
+        <xdr:cNvPr id="2" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1282,7 +1300,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 2"/>
+        <xdr:cNvPr id="4" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1354,7 +1378,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 2"/>
+        <xdr:cNvPr id="2" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1701,17 +1731,17 @@
   </sheetPr>
   <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A3" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39:F39"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40:F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.375" customWidth="1"/>
-    <col min="2" max="2" width="24.375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="53.375" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="53.42578125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="7" max="7" width="4.25" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
@@ -2088,225 +2118,231 @@
         <v>7</v>
       </c>
       <c r="D36" s="6"/>
-      <c r="E36" s="94" t="s">
+      <c r="E36" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="F36" s="94"/>
+      <c r="F36" s="84"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="30">
         <v>42639</v>
       </c>
-      <c r="C37" s="91" t="s">
+      <c r="C37" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="92"/>
-      <c r="E37" s="93" t="s">
+      <c r="D37" s="87"/>
+      <c r="E37" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="F37" s="93"/>
+      <c r="F37" s="85"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="30">
         <v>42648</v>
       </c>
-      <c r="C38" s="91" t="s">
+      <c r="C38" s="86" t="s">
         <v>97</v>
       </c>
-      <c r="D38" s="92"/>
-      <c r="E38" s="93" t="s">
+      <c r="D38" s="87"/>
+      <c r="E38" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="F38" s="93"/>
+      <c r="F38" s="85"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="30"/>
-      <c r="C39" s="91"/>
-      <c r="D39" s="92"/>
-      <c r="E39" s="93"/>
-      <c r="F39" s="93"/>
+      <c r="B39" s="30">
+        <v>42677</v>
+      </c>
+      <c r="C39" s="86" t="s">
+        <v>177</v>
+      </c>
+      <c r="D39" s="87"/>
+      <c r="E39" s="85" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="85"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="30"/>
-      <c r="C40" s="91"/>
-      <c r="D40" s="92"/>
-      <c r="E40" s="93"/>
-      <c r="F40" s="93"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="87"/>
+      <c r="E40" s="85"/>
+      <c r="F40" s="85"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="30"/>
-      <c r="C41" s="91"/>
-      <c r="D41" s="92"/>
-      <c r="E41" s="93"/>
-      <c r="F41" s="93"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="87"/>
+      <c r="E41" s="85"/>
+      <c r="F41" s="85"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="30"/>
-      <c r="C42" s="91"/>
-      <c r="D42" s="92"/>
-      <c r="E42" s="93"/>
-      <c r="F42" s="93"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="87"/>
+      <c r="E42" s="85"/>
+      <c r="F42" s="85"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="30"/>
-      <c r="C43" s="91"/>
-      <c r="D43" s="92"/>
-      <c r="E43" s="93"/>
-      <c r="F43" s="93"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="87"/>
+      <c r="E43" s="85"/>
+      <c r="F43" s="85"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="29"/>
-      <c r="C44" s="91"/>
-      <c r="D44" s="92"/>
-      <c r="E44" s="93"/>
-      <c r="F44" s="93"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="87"/>
+      <c r="E44" s="85"/>
+      <c r="F44" s="85"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="29"/>
-      <c r="C45" s="91"/>
-      <c r="D45" s="92"/>
-      <c r="E45" s="93"/>
-      <c r="F45" s="93"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="87"/>
+      <c r="E45" s="85"/>
+      <c r="F45" s="85"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="29"/>
-      <c r="C46" s="91"/>
-      <c r="D46" s="92"/>
-      <c r="E46" s="93"/>
-      <c r="F46" s="93"/>
+      <c r="C46" s="86"/>
+      <c r="D46" s="87"/>
+      <c r="E46" s="85"/>
+      <c r="F46" s="85"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="29"/>
-      <c r="C47" s="91"/>
-      <c r="D47" s="92"/>
-      <c r="E47" s="93"/>
-      <c r="F47" s="93"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="87"/>
+      <c r="E47" s="85"/>
+      <c r="F47" s="85"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="29"/>
-      <c r="C48" s="91"/>
-      <c r="D48" s="92"/>
-      <c r="E48" s="93"/>
-      <c r="F48" s="93"/>
+      <c r="C48" s="86"/>
+      <c r="D48" s="87"/>
+      <c r="E48" s="85"/>
+      <c r="F48" s="85"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="29"/>
-      <c r="C49" s="91"/>
-      <c r="D49" s="92"/>
-      <c r="E49" s="93"/>
-      <c r="F49" s="93"/>
+      <c r="C49" s="86"/>
+      <c r="D49" s="87"/>
+      <c r="E49" s="85"/>
+      <c r="F49" s="85"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="29"/>
-      <c r="C50" s="91"/>
-      <c r="D50" s="92"/>
-      <c r="E50" s="93"/>
-      <c r="F50" s="93"/>
+      <c r="C50" s="86"/>
+      <c r="D50" s="87"/>
+      <c r="E50" s="85"/>
+      <c r="F50" s="85"/>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="29"/>
-      <c r="C51" s="91"/>
-      <c r="D51" s="92"/>
-      <c r="E51" s="93"/>
-      <c r="F51" s="93"/>
+      <c r="C51" s="86"/>
+      <c r="D51" s="87"/>
+      <c r="E51" s="85"/>
+      <c r="F51" s="85"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="29"/>
-      <c r="C52" s="91"/>
-      <c r="D52" s="92"/>
-      <c r="E52" s="93"/>
-      <c r="F52" s="93"/>
+      <c r="C52" s="86"/>
+      <c r="D52" s="87"/>
+      <c r="E52" s="85"/>
+      <c r="F52" s="85"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="29"/>
-      <c r="C53" s="91"/>
-      <c r="D53" s="92"/>
-      <c r="E53" s="93"/>
-      <c r="F53" s="93"/>
+      <c r="C53" s="86"/>
+      <c r="D53" s="87"/>
+      <c r="E53" s="85"/>
+      <c r="F53" s="85"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="35"/>
-      <c r="C54" s="86"/>
-      <c r="D54" s="87"/>
-      <c r="E54" s="88"/>
-      <c r="F54" s="88"/>
+      <c r="C54" s="88"/>
+      <c r="D54" s="89"/>
+      <c r="E54" s="90"/>
+      <c r="F54" s="90"/>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="39"/>
-      <c r="C55" s="89"/>
-      <c r="D55" s="89"/>
-      <c r="E55" s="90"/>
-      <c r="F55" s="90"/>
+      <c r="C55" s="91"/>
+      <c r="D55" s="91"/>
+      <c r="E55" s="92"/>
+      <c r="F55" s="92"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="14"/>
-      <c r="C56" s="84"/>
-      <c r="D56" s="84"/>
-      <c r="E56" s="85"/>
-      <c r="F56" s="85"/>
+      <c r="C56" s="93"/>
+      <c r="D56" s="93"/>
+      <c r="E56" s="94"/>
+      <c r="F56" s="94"/>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="14"/>
-      <c r="C57" s="84"/>
-      <c r="D57" s="84"/>
-      <c r="E57" s="85"/>
-      <c r="F57" s="85"/>
+      <c r="C57" s="93"/>
+      <c r="D57" s="93"/>
+      <c r="E57" s="94"/>
+      <c r="F57" s="94"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="14"/>
-      <c r="C58" s="84"/>
-      <c r="D58" s="84"/>
-      <c r="E58" s="85"/>
-      <c r="F58" s="85"/>
+      <c r="C58" s="93"/>
+      <c r="D58" s="93"/>
+      <c r="E58" s="94"/>
+      <c r="F58" s="94"/>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="14"/>
-      <c r="C59" s="84"/>
-      <c r="D59" s="84"/>
-      <c r="E59" s="85"/>
-      <c r="F59" s="85"/>
+      <c r="C59" s="93"/>
+      <c r="D59" s="93"/>
+      <c r="E59" s="94"/>
+      <c r="F59" s="94"/>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="14"/>
-      <c r="C60" s="84"/>
-      <c r="D60" s="84"/>
-      <c r="E60" s="85"/>
-      <c r="F60" s="85"/>
+      <c r="C60" s="93"/>
+      <c r="D60" s="93"/>
+      <c r="E60" s="94"/>
+      <c r="F60" s="94"/>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="14"/>
-      <c r="C61" s="84"/>
-      <c r="D61" s="84"/>
-      <c r="E61" s="85"/>
-      <c r="F61" s="85"/>
+      <c r="C61" s="93"/>
+      <c r="D61" s="93"/>
+      <c r="E61" s="94"/>
+      <c r="F61" s="94"/>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="14"/>
-      <c r="C62" s="84"/>
-      <c r="D62" s="84"/>
-      <c r="E62" s="85"/>
-      <c r="F62" s="85"/>
+      <c r="C62" s="93"/>
+      <c r="D62" s="93"/>
+      <c r="E62" s="94"/>
+      <c r="F62" s="94"/>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="14"/>
-      <c r="C63" s="84"/>
-      <c r="D63" s="84"/>
-      <c r="E63" s="85"/>
-      <c r="F63" s="85"/>
+      <c r="C63" s="93"/>
+      <c r="D63" s="93"/>
+      <c r="E63" s="94"/>
+      <c r="F63" s="94"/>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="14"/>
-      <c r="C64" s="84"/>
-      <c r="D64" s="84"/>
-      <c r="E64" s="85"/>
-      <c r="F64" s="85"/>
+      <c r="C64" s="93"/>
+      <c r="D64" s="93"/>
+      <c r="E64" s="94"/>
+      <c r="F64" s="94"/>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="14"/>
-      <c r="C65" s="84"/>
-      <c r="D65" s="84"/>
-      <c r="E65" s="85"/>
-      <c r="F65" s="85"/>
+      <c r="C65" s="93"/>
+      <c r="D65" s="93"/>
+      <c r="E65" s="94"/>
+      <c r="F65" s="94"/>
     </row>
     <row r="88" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D88" t="b">
@@ -2316,53 +2352,6 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E59:F59"/>
     <mergeCell ref="C60:D60"/>
     <mergeCell ref="E60:F60"/>
     <mergeCell ref="C61:D61"/>
@@ -2375,6 +2364,53 @@
     <mergeCell ref="E63:F63"/>
     <mergeCell ref="C64:D64"/>
     <mergeCell ref="E64:F64"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2398,28 +2434,28 @@
       <selection pane="topRight" activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.375" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="13.75" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="15" customWidth="1"/>
-    <col min="5" max="5" width="6.75" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.375" style="15" customWidth="1"/>
-    <col min="8" max="8" width="18.125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="3" customWidth="1"/>
     <col min="9" max="9" width="18" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.25" style="3" customWidth="1"/>
-    <col min="13" max="13" width="24.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.25" style="3" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" style="3" customWidth="1"/>
     <col min="15" max="15" width="10" style="3" customWidth="1"/>
-    <col min="16" max="16" width="23.375" style="3" customWidth="1"/>
-    <col min="17" max="17" width="19.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.42578125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11" customWidth="1"/>
     <col min="19" max="19" width="22" customWidth="1"/>
-    <col min="20" max="20" width="15.375" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="25.5" x14ac:dyDescent="0.35">
@@ -5188,34 +5224,34 @@
   </sheetPr>
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A24" sqref="A24"/>
+      <selection pane="topRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
-    <col min="2" max="2" width="21.625" customWidth="1"/>
-    <col min="3" max="3" width="13.75" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="15" customWidth="1"/>
-    <col min="5" max="5" width="6.75" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" style="15" customWidth="1"/>
     <col min="8" max="8" width="17" style="15" customWidth="1"/>
-    <col min="9" max="9" width="18.125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" style="3" customWidth="1"/>
     <col min="10" max="10" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="19.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.25" style="3" customWidth="1"/>
-    <col min="14" max="14" width="24.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.25" style="3" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" style="3" customWidth="1"/>
     <col min="16" max="16" width="10" style="3" customWidth="1"/>
-    <col min="17" max="17" width="23.375" style="3" customWidth="1"/>
-    <col min="18" max="18" width="19.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.42578125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11" customWidth="1"/>
     <col min="20" max="20" width="22" customWidth="1"/>
-    <col min="21" max="21" width="15.375" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="25.5" x14ac:dyDescent="0.35">
@@ -5870,9 +5906,15 @@
       <c r="Y24"/>
     </row>
     <row r="25" spans="1:25" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="61"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
+      <c r="A25" s="61" t="s">
+        <v>175</v>
+      </c>
+      <c r="B25" s="96" t="s">
+        <v>176</v>
+      </c>
+      <c r="C25" s="29">
+        <v>647204</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
@@ -6126,11 +6168,14 @@
   <mergeCells count="1">
     <mergeCell ref="A4:R4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B25" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="46" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="46" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;F   &amp;A</oddHeader>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>